<commit_message>
Finish write up and readme
</commit_message>
<xml_diff>
--- a/project6_cs475/Project6.xlsx
+++ b/project6_cs475/Project6.xlsx
@@ -110,8 +110,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -137,7 +143,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -147,6 +153,9 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -156,6 +165,9 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,11 +381,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="929813376"/>
-        <c:axId val="1030179488"/>
+        <c:axId val="1110866032"/>
+        <c:axId val="1029337200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="929813376"/>
+        <c:axId val="1110866032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030179488"/>
+        <c:crossAx val="1029337200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -424,7 +436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1030179488"/>
+        <c:axId val="1029337200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="929813376"/>
+        <c:crossAx val="1110866032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -744,11 +756,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1108388256"/>
-        <c:axId val="1108390304"/>
+        <c:axId val="1062084592"/>
+        <c:axId val="928803120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1108388256"/>
+        <c:axId val="1062084592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,7 +803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1108390304"/>
+        <c:crossAx val="928803120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -799,7 +811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1108390304"/>
+        <c:axId val="928803120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,6 +831,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -849,7 +862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1108388256"/>
+        <c:crossAx val="1062084592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1128,11 +1141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1108473872"/>
-        <c:axId val="1108475920"/>
+        <c:axId val="1074561344"/>
+        <c:axId val="1074562704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1108473872"/>
+        <c:axId val="1074561344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1108475920"/>
+        <c:crossAx val="1074562704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1183,7 +1196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1108475920"/>
+        <c:axId val="1074562704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1246,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1108473872"/>
+        <c:crossAx val="1074561344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1503,11 +1516,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1061337680"/>
-        <c:axId val="927931344"/>
+        <c:axId val="1029993920"/>
+        <c:axId val="1029995280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1061337680"/>
+        <c:axId val="1029993920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1550,7 +1563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="927931344"/>
+        <c:crossAx val="1029995280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1558,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="927931344"/>
+        <c:axId val="1029995280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1609,7 +1622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1061337680"/>
+        <c:crossAx val="1029993920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1798,6 +1811,45 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet3!$D$2:$D$11</c:f>
@@ -1849,16 +1901,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1074319296"/>
-        <c:axId val="1031742624"/>
+        <c:axId val="1074461104"/>
+        <c:axId val="1060092464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1074319296"/>
+        <c:axId val="1074461104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1895,7 +1948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031742624"/>
+        <c:crossAx val="1060092464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1903,7 +1956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1031742624"/>
+        <c:axId val="1060092464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +2007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1074319296"/>
+        <c:crossAx val="1074461104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2146,6 +2199,39 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$82:$A$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet3!$D$82:$D$89</c:f>
@@ -2191,16 +2277,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1111008640"/>
-        <c:axId val="1111010688"/>
+        <c:axId val="1074053616"/>
+        <c:axId val="1074055664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1111008640"/>
+        <c:axId val="1074053616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2237,7 +2324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1111010688"/>
+        <c:crossAx val="1074055664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2245,7 +2332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1111010688"/>
+        <c:axId val="1074055664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2296,7 +2383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1111008640"/>
+        <c:crossAx val="1074053616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6095,8 +6182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7448,7 +7535,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>